<commit_message>
Add CBRE and Balfour Beatty PLC data.
Signed-off-by: MichaelTiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220927 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220927 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR-MichaelTiemannOSC/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97097308-073E-C34D-A2AE-6FF7383B4C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B068B0-BD3A-3941-8575-83DF17DED469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11700" windowWidth="71800" windowHeight="26600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="11700" windowWidth="48440" windowHeight="26600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="1" r:id="rId1"/>
@@ -383,6 +383,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="AT76" authorId="1" shapeId="0" xr:uid="{16EB716C-AB4A-BE4F-AD78-A8E7300F26BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>These are all in GBP!</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -712,7 +745,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="428">
   <si>
     <t>company_name</t>
   </si>
@@ -2192,22 +2225,34 @@
     <t>Tpkm</t>
   </si>
   <si>
-    <t>Fictional Realty</t>
-  </si>
-  <si>
-    <t>TIE0001</t>
-  </si>
-  <si>
-    <t>US0001</t>
-  </si>
-  <si>
     <t>Commercial Buildings</t>
   </si>
   <si>
-    <t>g CO2/m**2</t>
-  </si>
-  <si>
-    <t>thousand m**2</t>
+    <t>Balfour Beatty</t>
+  </si>
+  <si>
+    <t>CT4UIJ3TUKGYYHMENQ17</t>
+  </si>
+  <si>
+    <t>GB0000961622</t>
+  </si>
+  <si>
+    <t>Construction Buildings</t>
+  </si>
+  <si>
+    <t>CBRE</t>
+  </si>
+  <si>
+    <t>52990016II9MJ2OSWA10</t>
+  </si>
+  <si>
+    <t>US12504L1098</t>
+  </si>
+  <si>
+    <t>ft**2</t>
+  </si>
+  <si>
+    <t>kg CO2/ft**2</t>
   </si>
 </sst>
 </file>
@@ -3967,10 +4012,10 @@
   <dimension ref="A1:AZ82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P77" sqref="P77"/>
+      <selection pane="bottomRight" activeCell="AQ77" sqref="AQ77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -13691,22 +13736,20 @@
     </row>
     <row r="76" spans="1:50">
       <c r="A76" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C76" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D76" t="s">
-        <v>54</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E76" s="1"/>
       <c r="F76" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>56</v>
@@ -13717,130 +13760,250 @@
       <c r="I76" s="3">
         <v>44561</v>
       </c>
-      <c r="J76">
-        <v>1</v>
-      </c>
-      <c r="K76">
-        <v>1</v>
-      </c>
-      <c r="L76">
-        <v>1</v>
-      </c>
-      <c r="M76">
-        <v>1</v>
-      </c>
-      <c r="N76">
-        <v>1</v>
+      <c r="J76" s="22">
+        <v>2260000000</v>
+      </c>
+      <c r="K76" s="22">
+        <v>9690000000</v>
+      </c>
+      <c r="L76" s="22">
+        <v>1810000000</v>
+      </c>
+      <c r="M76" s="22">
+        <f>L76+1110000000</f>
+        <v>2920000000</v>
+      </c>
+      <c r="N76" s="22">
+        <v>4846000000</v>
       </c>
       <c r="O76" t="s">
         <v>58</v>
       </c>
       <c r="P76" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q76">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R76">
-        <v>49</v>
+        <v>170937</v>
       </c>
       <c r="S76">
-        <v>48</v>
+        <v>175065</v>
       </c>
       <c r="T76">
-        <v>47</v>
+        <v>167071</v>
       </c>
       <c r="U76">
-        <v>46</v>
+        <v>162816</v>
       </c>
       <c r="V76">
-        <v>45</v>
-      </c>
-      <c r="X76">
-        <v>1000</v>
+        <v>199002</v>
       </c>
       <c r="Y76">
-        <v>990</v>
+        <v>71170</v>
       </c>
       <c r="Z76">
-        <v>980</v>
+        <v>49365</v>
       </c>
       <c r="AA76">
-        <v>970</v>
+        <v>43561</v>
       </c>
       <c r="AB76">
-        <v>960</v>
+        <v>42701</v>
       </c>
       <c r="AC76">
-        <v>950</v>
-      </c>
-      <c r="AE76" s="19">
-        <f t="shared" si="60"/>
-        <v>1050</v>
+        <v>41779</v>
+      </c>
+      <c r="AE76" s="19" t="str">
+        <f>IF(ISBLANK(Q76),IF(ISBLANK(X76),"",X76),Q76+X76)</f>
+        <v/>
       </c>
       <c r="AF76" s="19">
-        <f t="shared" si="60"/>
-        <v>1039</v>
+        <f>IF(ISBLANK(R76),IF(ISBLANK(Y76),"",Y76),R76+Y76)</f>
+        <v>242107</v>
       </c>
       <c r="AG76" s="19">
-        <f t="shared" si="60"/>
-        <v>1028</v>
+        <f>IF(ISBLANK(S76),IF(ISBLANK(Z76),"",Z76),S76+Z76)</f>
+        <v>224430</v>
       </c>
       <c r="AH76" s="19">
-        <f t="shared" si="60"/>
-        <v>1017</v>
+        <f>IF(ISBLANK(T76),IF(ISBLANK(AA76),"",AA76),T76+AA76)</f>
+        <v>210632</v>
       </c>
       <c r="AI76" s="19">
-        <f t="shared" si="60"/>
-        <v>1006</v>
+        <f>IF(ISBLANK(U76),IF(ISBLANK(AB76),"",AB76),U76+AB76)</f>
+        <v>205517</v>
       </c>
       <c r="AJ76" s="19">
-        <f t="shared" si="60"/>
-        <v>995</v>
+        <f>IF(ISBLANK(V76),IF(ISBLANK(AC76),"",AC76),V76+AC76)</f>
+        <v>240781</v>
       </c>
       <c r="AK76" s="19" t="str">
         <f t="shared" si="60"/>
         <v/>
       </c>
-      <c r="AL76">
-        <v>100</v>
-      </c>
-      <c r="AM76">
-        <v>99</v>
-      </c>
-      <c r="AN76">
-        <v>98</v>
-      </c>
-      <c r="AO76">
-        <v>97</v>
-      </c>
-      <c r="AP76">
-        <v>96</v>
-      </c>
-      <c r="AQ76">
-        <v>95</v>
-      </c>
-      <c r="AS76">
-        <v>10</v>
-      </c>
-      <c r="AT76">
-        <v>11</v>
-      </c>
-      <c r="AU76">
-        <v>12</v>
-      </c>
-      <c r="AV76">
-        <v>13</v>
-      </c>
-      <c r="AW76">
-        <v>14</v>
-      </c>
-      <c r="AX76">
-        <v>15</v>
+      <c r="AT76" s="22">
+        <v>8234000000</v>
+      </c>
+      <c r="AU76" s="22">
+        <v>7802000000</v>
+      </c>
+      <c r="AV76" s="22">
+        <v>8405000000</v>
+      </c>
+      <c r="AW76" s="22">
+        <v>8587000000</v>
+      </c>
+      <c r="AX76" s="22">
+        <v>8280000000</v>
       </c>
     </row>
     <row r="77" spans="1:50">
+      <c r="A77" t="s">
+        <v>423</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C77" t="s">
+        <v>425</v>
+      </c>
+      <c r="D77" t="s">
+        <v>54</v>
+      </c>
       <c r="E77"/>
+      <c r="F77" t="s">
+        <v>418</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H77" t="s">
+        <v>57</v>
+      </c>
+      <c r="I77" s="3">
+        <v>44561</v>
+      </c>
+      <c r="J77" s="22">
+        <v>36310000000</v>
+      </c>
+      <c r="K77" s="22">
+        <v>27740000000</v>
+      </c>
+      <c r="L77" s="22">
+        <v>37840000000</v>
+      </c>
+      <c r="M77" s="22">
+        <f>L77+1190000000</f>
+        <v>39030000000</v>
+      </c>
+      <c r="N77" s="22">
+        <v>22073000000</v>
+      </c>
+      <c r="O77" t="s">
+        <v>58</v>
+      </c>
+      <c r="P77" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q77">
+        <v>63414</v>
+      </c>
+      <c r="R77">
+        <v>46057</v>
+      </c>
+      <c r="S77">
+        <v>46069</v>
+      </c>
+      <c r="T77">
+        <v>58770</v>
+      </c>
+      <c r="U77">
+        <v>60379</v>
+      </c>
+      <c r="V77">
+        <v>46251</v>
+      </c>
+      <c r="X77">
+        <v>29678</v>
+      </c>
+      <c r="Y77">
+        <v>25010</v>
+      </c>
+      <c r="Z77">
+        <v>24439</v>
+      </c>
+      <c r="AA77">
+        <v>28020</v>
+      </c>
+      <c r="AB77">
+        <v>22644</v>
+      </c>
+      <c r="AC77">
+        <v>19847</v>
+      </c>
+      <c r="AE77" s="19">
+        <f>IF(ISBLANK(Q77),IF(ISBLANK(X77),"",X77),Q77+X77)</f>
+        <v>93092</v>
+      </c>
+      <c r="AF77" s="19">
+        <f>IF(ISBLANK(R77),IF(ISBLANK(Y77),"",Y77),R77+Y77)</f>
+        <v>71067</v>
+      </c>
+      <c r="AG77" s="19">
+        <f>IF(ISBLANK(S77),IF(ISBLANK(Z77),"",Z77),S77+Z77)</f>
+        <v>70508</v>
+      </c>
+      <c r="AH77" s="19">
+        <f>IF(ISBLANK(T77),IF(ISBLANK(AA77),"",AA77),T77+AA77)</f>
+        <v>86790</v>
+      </c>
+      <c r="AI77" s="19">
+        <f>IF(ISBLANK(U77),IF(ISBLANK(AB77),"",AB77),U77+AB77)</f>
+        <v>83023</v>
+      </c>
+      <c r="AJ77" s="19">
+        <f>IF(ISBLANK(V77),IF(ISBLANK(AC77),"",AC77),V77+AC77)</f>
+        <v>66098</v>
+      </c>
+      <c r="AK77" s="19" t="str">
+        <f>IF(ISBLANK(W77),IF(ISBLANK(AD77),"",AD77),W77+AD77)</f>
+        <v/>
+      </c>
+      <c r="AL77">
+        <v>16954</v>
+      </c>
+      <c r="AM77">
+        <v>18626</v>
+      </c>
+      <c r="AN77">
+        <v>19984</v>
+      </c>
+      <c r="AO77">
+        <v>58307929</v>
+      </c>
+      <c r="AP77">
+        <v>54684733</v>
+      </c>
+      <c r="AQ77">
+        <v>89168768</v>
+      </c>
+      <c r="AS77" s="22">
+        <v>5300000000</v>
+      </c>
+      <c r="AT77" s="22">
+        <v>5500000000</v>
+      </c>
+      <c r="AU77" s="22">
+        <v>6000000000</v>
+      </c>
+      <c r="AV77" s="22">
+        <v>6800000000</v>
+      </c>
+      <c r="AW77" s="22">
+        <v>7000000000</v>
+      </c>
+      <c r="AX77" s="22">
+        <v>7100000000</v>
+      </c>
     </row>
     <row r="78" spans="1:50">
       <c r="E78"/>
@@ -13877,13 +14040,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
-      <selection pane="bottomRight" activeCell="K108" sqref="K108"/>
+      <selection pane="bottomRight" activeCell="A110" sqref="A110:C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -18199,22 +18362,22 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C108" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D108" t="s">
         <v>54</v>
       </c>
       <c r="E108" s="30">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="F108" s="30" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G108" t="s">
         <v>294</v>
@@ -18223,20 +18386,102 @@
         <v>2020</v>
       </c>
       <c r="I108" s="33">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="J108">
-        <f>'ITR input data'!AE76</f>
-        <v>1050</v>
+        <v>357983</v>
       </c>
       <c r="K108" t="s">
-        <v>422</v>
+        <v>58</v>
       </c>
       <c r="L108">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="M108" s="43">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13">
+      <c r="A109" t="s">
+        <v>423</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C109" t="s">
+        <v>425</v>
+      </c>
+      <c r="D109" t="s">
+        <v>54</v>
+      </c>
+      <c r="E109" s="30">
+        <v>2050</v>
+      </c>
+      <c r="F109" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="G109" t="s">
+        <v>294</v>
+      </c>
+      <c r="H109">
+        <v>2020</v>
+      </c>
+      <c r="I109" s="33">
+        <v>2019</v>
+      </c>
+      <c r="J109">
+        <v>87198</v>
+      </c>
+      <c r="K109" t="s">
+        <v>58</v>
+      </c>
+      <c r="L109">
+        <v>2035</v>
+      </c>
+      <c r="M109" s="43">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13">
+      <c r="A110" t="s">
+        <v>423</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C110" t="s">
+        <v>425</v>
+      </c>
+      <c r="D110" t="s">
+        <v>54</v>
+      </c>
+      <c r="E110" s="30">
+        <v>2050</v>
+      </c>
+      <c r="F110" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="G110" t="s">
+        <v>300</v>
+      </c>
+      <c r="H110">
+        <v>2020</v>
+      </c>
+      <c r="I110" s="33">
+        <v>2019</v>
+      </c>
+      <c r="J110">
+        <f>0.01865*1000</f>
+        <v>18.649999999999999</v>
+      </c>
+      <c r="K110" t="s">
+        <v>427</v>
+      </c>
+      <c r="L110">
+        <v>2035</v>
+      </c>
+      <c r="M110" s="43">
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>
@@ -19479,10 +19724,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -19524,7 +19769,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>179862180</v>
+        <v>60311111</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -19542,7 +19787,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E67" ca="1" si="0">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>137285676</v>
+        <v>149142976</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -19560,7 +19805,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>205657907</v>
+        <v>177999462</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -19578,7 +19823,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>110458106</v>
+        <v>146111295</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -19596,7 +19841,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>53540055</v>
+        <v>109540802</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -19614,7 +19859,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>93911338</v>
+        <v>170383032</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -19632,7 +19877,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>101650080</v>
+        <v>108589923</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -19650,7 +19895,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>184958915</v>
+        <v>102312964</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -19668,7 +19913,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>199157436</v>
+        <v>86269376</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -19686,7 +19931,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>55980320</v>
+        <v>82735928</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -19704,7 +19949,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>143182254</v>
+        <v>84248391</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -19722,7 +19967,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>47642409</v>
+        <v>274102374</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -19740,7 +19985,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>154545400</v>
+        <v>76642360</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -19758,7 +20003,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>98866152</v>
+        <v>94716144</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -19776,7 +20021,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>198114203</v>
+        <v>85299705</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -19794,7 +20039,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>97111324</v>
+        <v>243013288</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -19812,7 +20057,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>195730457</v>
+        <v>128911797</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -19830,7 +20075,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>88201050</v>
+        <v>158656944</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -19848,7 +20093,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>173598040</v>
+        <v>108959076</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -19866,7 +20111,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>85840056</v>
+        <v>66377165</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -19884,7 +20129,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>155612699</v>
+        <v>158545194</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -19902,7 +20147,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>174324990</v>
+        <v>56594197</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -19920,7 +20165,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>82029584</v>
+        <v>170949534</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -19938,7 +20183,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>107760475</v>
+        <v>111861590</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -19956,7 +20201,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>282522640</v>
+        <v>62412768</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -19974,7 +20219,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>175845031</v>
+        <v>103646520</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -19992,7 +20237,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>78528528</v>
+        <v>62387512</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -20010,7 +20255,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>150413760</v>
+        <v>125263890</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -20028,7 +20273,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>57296025</v>
+        <v>106969476</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -20046,7 +20291,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>75146000</v>
+        <v>77872662</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -20064,7 +20309,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>80172170</v>
+        <v>157351700</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -20082,7 +20327,7 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>72473967</v>
+        <v>60670420</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -20100,7 +20345,7 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>61561164</v>
+        <v>135327830</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -20118,7 +20363,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>184101928</v>
+        <v>199381392</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -20136,7 +20381,7 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>237562272</v>
+        <v>134305857</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -20154,7 +20399,7 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>100229828</v>
+        <v>154428480</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -20172,7 +20417,7 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>91373184</v>
+        <v>141312738</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -20190,7 +20435,7 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="0"/>
-        <v>72181460</v>
+        <v>227460920</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -20208,7 +20453,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="0"/>
-        <v>120870010</v>
+        <v>98718116</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -20226,7 +20471,7 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="0"/>
-        <v>203989248</v>
+        <v>212091119</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -20244,7 +20489,7 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="0"/>
-        <v>75070336</v>
+        <v>62502125</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -20262,7 +20507,7 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="0"/>
-        <v>164985964</v>
+        <v>239175417</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -20280,7 +20525,7 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="0"/>
-        <v>162121800</v>
+        <v>117405450</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -20298,7 +20543,7 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="0"/>
-        <v>110321620</v>
+        <v>179066862</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -20316,7 +20561,7 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="0"/>
-        <v>196548141</v>
+        <v>243488040</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -20334,7 +20579,7 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="0"/>
-        <v>184521242</v>
+        <v>235806480</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -20352,7 +20597,7 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="0"/>
-        <v>153289800</v>
+        <v>41687382</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -20370,7 +20615,7 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="0"/>
-        <v>149872852</v>
+        <v>169466016</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -20388,7 +20633,7 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="0"/>
-        <v>42208712</v>
+        <v>105117452</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -20406,7 +20651,7 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="0"/>
-        <v>34416975</v>
+        <v>59770452</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -20424,7 +20669,7 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="0"/>
-        <v>108336954</v>
+        <v>260477340</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -20442,7 +20687,7 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="0"/>
-        <v>107325396</v>
+        <v>217416231</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -20460,7 +20705,7 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="0"/>
-        <v>238022610</v>
+        <v>176255753</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -20478,7 +20723,7 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="0"/>
-        <v>91411040</v>
+        <v>75214200</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -20496,7 +20741,7 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="0"/>
-        <v>111100878</v>
+        <v>176599773</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -20514,7 +20759,7 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="0"/>
-        <v>250924328</v>
+        <v>73529160</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -20532,7 +20777,7 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="0"/>
-        <v>187000890</v>
+        <v>75163012</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -20550,7 +20795,7 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="0"/>
-        <v>140207463</v>
+        <v>73872636</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -20568,7 +20813,7 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="0"/>
-        <v>111206909</v>
+        <v>106615189</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -20586,7 +20831,7 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="0"/>
-        <v>121145312</v>
+        <v>142345500</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -20604,7 +20849,7 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="0"/>
-        <v>110535004</v>
+        <v>93686336</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -20622,7 +20867,7 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="0"/>
-        <v>277687201</v>
+        <v>177322387</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -20640,7 +20885,7 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="0"/>
-        <v>89881190</v>
+        <v>158584236</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -20658,7 +20903,7 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="0"/>
-        <v>101850624</v>
+        <v>133649040</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -20676,7 +20921,7 @@
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="0"/>
-        <v>191225133</v>
+        <v>103636994</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -20694,7 +20939,7 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="0"/>
-        <v>54360320</v>
+        <v>110347536</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -20711,8 +20956,8 @@
         <v>261</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E76" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>205502882</v>
+        <f t="shared" ref="E68:E77" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
+        <v>63074720</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -20730,7 +20975,7 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="1"/>
-        <v>262971153</v>
+        <v>57436140</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -20748,7 +20993,7 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="1"/>
-        <v>100831536</v>
+        <v>260385605</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -20766,7 +21011,7 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="1"/>
-        <v>125252400</v>
+        <v>147708036</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -20784,7 +21029,7 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="1"/>
-        <v>259095168</v>
+        <v>34522810</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -20802,7 +21047,7 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="1"/>
-        <v>179523893</v>
+        <v>124145028</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -20820,7 +21065,7 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="1"/>
-        <v>99777300</v>
+        <v>92207874</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -20838,25 +21083,43 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="1"/>
-        <v>96659416</v>
+        <v>163106028</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C76" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D76" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="1"/>
-        <v>105795263</v>
+        <v>178385184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>423</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C77" t="s">
+        <v>425</v>
+      </c>
+      <c r="D77" t="s">
+        <v>425</v>
+      </c>
+      <c r="E77">
+        <f t="shared" ca="1" si="1"/>
+        <v>239430800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up release issues
Bump various version numbers of libraries we use in requirements.txt.  Also fix a latent data error in one of the two 20220927 excel spreadsheets.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220927 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220927 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B00BD2C-BC86-8F42-B440-EB2D9A420E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFA045B-994F-3742-B784-D5EF4B91AC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11700" windowWidth="48440" windowHeight="26600" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="11700" windowWidth="48440" windowHeight="26600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="1" r:id="rId1"/>
@@ -14009,11 +14009,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
-      <selection pane="bottomRight" activeCell="A110" sqref="A110:C110"/>
+      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -15394,7 +15394,7 @@
         <v>299</v>
       </c>
       <c r="H35">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="I35" s="31">
         <v>2000</v>
@@ -19693,7 +19693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E77"/>
     </sheetView>
   </sheetViews>

</xml_diff>